<commit_message>
Excel File Updated With Change Details
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\Alam-Sher-Khan\neocortexapi-classification\My Analysis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0445EFD-EC59-4528-9173-AFC92880865F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,43 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+  <si>
+    <t>Local Area Density</t>
+  </si>
+  <si>
+    <t>Potential Radius</t>
+  </si>
+  <si>
+    <t>Local/Global Inhibition</t>
+  </si>
+  <si>
+    <t>NumActiveColumnsPerInhArea</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Exp 6</t>
+  </si>
+  <si>
+    <t>Exp 7</t>
+  </si>
+  <si>
+    <t>Result Image Name</t>
+  </si>
+  <si>
+    <t>Experiment Folder</t>
+  </si>
+  <si>
+    <t>Exp 6.png</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,15 +70,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +92,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +399,191 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Excel File Updated With Exp 8 Parameters Changes
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\Alam-Sher-Khan\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0445EFD-EC59-4528-9173-AFC92880865F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6408528-BA65-4E52-83F7-5F25E9D80730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>Exp 6.png</t>
+  </si>
+  <si>
+    <t>Exp 7.png</t>
+  </si>
+  <si>
+    <t>Exp 8</t>
+  </si>
+  <si>
+    <t>Exp 8.png</t>
   </si>
 </sst>
 </file>
@@ -403,7 +412,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,16 +481,28 @@
       <c r="E3" s="3">
         <v>-1</v>
       </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>10</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="3">
         <v>-1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Excel Updated with Exp 9 HTM Parameters
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\Alam-Sher-Khan\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6408528-BA65-4E52-83F7-5F25E9D80730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2F685A-0D9D-4C51-8D44-58C266D44E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Exp 8.png</t>
+  </si>
+  <si>
+    <t>Exp 9</t>
+  </si>
+  <si>
+    <t>Exp 9.png</t>
   </si>
 </sst>
 </file>
@@ -412,7 +418,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,14 +512,23 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="3">
         <v>-1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Excel File Updated with Exp 10 HTM Parameters
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\Alam-Sher-Khan\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2F685A-0D9D-4C51-8D44-58C266D44E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE61AF20-6136-44C0-A2F9-477C9C6A5F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Exp 9.png</t>
+  </si>
+  <si>
+    <t>Exp 10</t>
+  </si>
+  <si>
+    <t>Exp 10.png</t>
   </si>
 </sst>
 </file>
@@ -532,14 +538,23 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
       <c r="D6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="3">
         <v>-1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Excel File Updated with Exp 11 HTM Parameters
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\Alam-Sher-Khan\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE61AF20-6136-44C0-A2F9-477C9C6A5F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC82164-2A71-4453-81FA-72676EC58A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Exp 10.png</t>
+  </si>
+  <si>
+    <t>Exp 11</t>
+  </si>
+  <si>
+    <t>Exp11.png</t>
   </si>
 </sst>
 </file>
@@ -424,7 +430,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,14 +564,23 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
       <c r="D7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="3">
         <v>-1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Excel File Updated with Exp 12 Parameters
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\Alam-Sher-Khan\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC82164-2A71-4453-81FA-72676EC58A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B4DD51-D1C3-450C-8F78-7A8CEC29928B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -81,7 +81,13 @@
     <t>Exp 11</t>
   </si>
   <si>
-    <t>Exp11.png</t>
+    <t>Exp 12</t>
+  </si>
+  <si>
+    <t>Exp 12.png</t>
+  </si>
+  <si>
+    <t>Exp 11.png</t>
   </si>
 </sst>
 </file>
@@ -430,7 +436,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,18 +586,27 @@
         <v>-1</v>
       </c>
       <c r="F7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
       <c r="D8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="3">
         <v>-1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Excel file updated with Exp 13 HTM Parameters
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\Alam-Sher-Khan\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B4DD51-D1C3-450C-8F78-7A8CEC29928B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215C2C83-6024-45F7-8662-3816E3450D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Exp 11.png</t>
+  </si>
+  <si>
+    <t>Exp 13</t>
+  </si>
+  <si>
+    <t>Exp 13.png</t>
   </si>
 </sst>
 </file>
@@ -436,7 +442,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,14 +616,23 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
       <c r="D9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="3">
         <v>-1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Excel File Updated with Exp 14 HTM Parameters
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\Alam-Sher-Khan\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215C2C83-6024-45F7-8662-3816E3450D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05ACA1FE-4F40-4DE3-97F8-490ED20442C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>Exp 13.png</t>
+  </si>
+  <si>
+    <t>Exp 14</t>
+  </si>
+  <si>
+    <t>Exp 14.png</t>
   </si>
 </sst>
 </file>
@@ -442,7 +448,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F14" sqref="F14:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,14 +642,23 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
       <c r="D10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="3">
         <v>-1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Excel file updated with Exp15 HTM Parameters
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\Alam-Sher-Khan\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05ACA1FE-4F40-4DE3-97F8-490ED20442C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA33F105-AE3B-4730-AC2D-99C1E6AD5ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Exp 14.png</t>
+  </si>
+  <si>
+    <t>Exp 15</t>
+  </si>
+  <si>
+    <t>Exp 15.png</t>
   </si>
 </sst>
 </file>
@@ -448,7 +454,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14:F15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,14 +668,23 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
       <c r="D11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="3">
         <v>-1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Excel File Updated with Exp 16 HTM Parameters
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\Alam-Sher-Khan\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA33F105-AE3B-4730-AC2D-99C1E6AD5ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFC0697-A348-4E73-84D4-A57DF35EA0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Exp 15.png</t>
+  </si>
+  <si>
+    <t>Exp 16</t>
+  </si>
+  <si>
+    <t>Exp 16.png</t>
   </si>
 </sst>
 </file>
@@ -454,7 +460,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,14 +694,23 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
       <c r="D12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E12" s="3">
         <v>-1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Excel File Updated with Exp 17 HTM Parameters
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\Alam-Sher-Khan\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFC0697-A348-4E73-84D4-A57DF35EA0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76096B1-AA92-4E49-8EF0-A22D34F9B021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Exp 16.png</t>
+  </si>
+  <si>
+    <t>Exp 17</t>
+  </si>
+  <si>
+    <t>Exp 17.png</t>
   </si>
 </sst>
 </file>
@@ -460,7 +466,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,14 +720,23 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="A13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
       <c r="D13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="3">
         <v>-1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel File Updated with Exp 18 HTM Parameters
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\Alam-Sher-Khan\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76096B1-AA92-4E49-8EF0-A22D34F9B021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25620C54-AB81-43AE-ADF0-83ADC9BEB3E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Exp 17.png</t>
+  </si>
+  <si>
+    <t>Exp 18</t>
+  </si>
+  <si>
+    <t>Exp 18.png</t>
   </si>
 </sst>
 </file>
@@ -463,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,6 +745,26 @@
         <v>30</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Excel File Updated with Exp 19 HTM Parameters
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\Alam-Sher-Khan\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25620C54-AB81-43AE-ADF0-83ADC9BEB3E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71565EFD-093D-4F38-8DD9-2F43BEA9206F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Exp 18.png</t>
+  </si>
+  <si>
+    <t>Exp 19</t>
+  </si>
+  <si>
+    <t>Exp 19.png</t>
   </si>
 </sst>
 </file>
@@ -469,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,6 +771,26 @@
         <v>32</v>
       </c>
     </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Upadted Excel with Exp 20 HTM Parameters
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\Alam-Sher-Khan\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71565EFD-093D-4F38-8DD9-2F43BEA9206F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBFB044-60BC-4C72-86E9-1799B82559C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>Exp 19.png</t>
+  </si>
+  <si>
+    <t>Exp 20</t>
+  </si>
+  <si>
+    <t>Exp 20.png</t>
   </si>
 </sst>
 </file>
@@ -475,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +777,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
@@ -789,6 +795,26 @@
       </c>
       <c r="F15" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel File Updated with Exp 21 HTM Parameters
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\Alam-Sher-Khan\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBFB044-60BC-4C72-86E9-1799B82559C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2F3926-35E6-425F-A929-1754192B4EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>Exp 20.png</t>
+  </si>
+  <si>
+    <t>Exp 21</t>
+  </si>
+  <si>
+    <t>Exp 21.png</t>
   </si>
 </sst>
 </file>
@@ -481,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,6 +823,26 @@
         <v>36</v>
       </c>
     </row>
+    <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Excel File updated with Exp22 HTM Parameters
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\Alam-Sher-Khan\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2F3926-35E6-425F-A929-1754192B4EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1702A6F-C4AD-4E3B-9FF8-A81AC81FBAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>Exp 21.png</t>
+  </si>
+  <si>
+    <t>Exp 22</t>
+  </si>
+  <si>
+    <t>Exp 22.png</t>
   </si>
 </sst>
 </file>
@@ -487,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,6 +849,26 @@
         <v>38</v>
       </c>
     </row>
+    <row r="18" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
HTM Changes updated in Excel
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\Alam-Sher-Khan\neocortexapi-classification\My Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1702A6F-C4AD-4E3B-9FF8-A81AC81FBAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3339F66F-F32E-4A38-818C-1A10D0CC25E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Exp 22.png</t>
+  </si>
+  <si>
+    <t>Exp 23</t>
+  </si>
+  <si>
+    <t>Exp 23.png</t>
   </si>
 </sst>
 </file>
@@ -493,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,6 +875,26 @@
         <v>40</v>
       </c>
     </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Excel File Updated with Exp 24 HTM Parameters
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3339F66F-F32E-4A38-818C-1A10D0CC25E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530AEF11-8373-41FC-A183-96606EC4F565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Exp 23.png</t>
+  </si>
+  <si>
+    <t>Exp 24.png</t>
   </si>
 </sst>
 </file>
@@ -499,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,6 +898,26 @@
         <v>42</v>
       </c>
     </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Excel File Update with Exp 25 htm parameters
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530AEF11-8373-41FC-A183-96606EC4F565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE77646-1DA9-463B-8876-C752D63AA8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -157,6 +157,15 @@
   </si>
   <si>
     <t>Exp 24.png</t>
+  </si>
+  <si>
+    <t>Exp 24</t>
+  </si>
+  <si>
+    <t>Exp 25</t>
+  </si>
+  <si>
+    <t>Exp 25.png</t>
   </si>
 </sst>
 </file>
@@ -502,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,7 +909,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B20" s="3">
         <v>0.2</v>
@@ -916,6 +925,26 @@
       </c>
       <c r="F20" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Experimenting with changed dataset
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE77646-1DA9-463B-8876-C752D63AA8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB716D3D-E865-4EF9-80AB-6290F3138011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Exp 25.png</t>
+  </si>
+  <si>
+    <t>Exp 26</t>
   </si>
 </sst>
 </file>
@@ -222,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -231,6 +234,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,6 +951,24 @@
         <v>46</v>
       </c>
     </row>
+    <row r="22" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C23" s="3">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="3">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Excel File Updated with Exp 26 and 27 Parameters
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB716D3D-E865-4EF9-80AB-6290F3138011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38042553-5131-4A91-BE55-64F7B45CCF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -169,6 +169,15 @@
   </si>
   <si>
     <t>Exp 26</t>
+  </si>
+  <si>
+    <t>Exp 27</t>
+  </si>
+  <si>
+    <t>Exp 26.png</t>
+  </si>
+  <si>
+    <t>Exp 27.png</t>
   </si>
 </sst>
 </file>
@@ -515,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,6 +977,29 @@
       <c r="E23" s="3">
         <v>-1</v>
       </c>
+      <c r="F23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="C24" s="3">
+        <v>30</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Exp 28 for Digits 0,1,9
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC59E262-9DF3-4FAD-ABAE-934F18D6C889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9D5C00-D220-400D-876F-BC7084F6CBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -193,6 +193,21 @@
   </si>
   <si>
     <t>Macro 2 wrt 0</t>
+  </si>
+  <si>
+    <t>Exp 28</t>
+  </si>
+  <si>
+    <t>Exp 28.png</t>
+  </si>
+  <si>
+    <t>Micro 9</t>
+  </si>
+  <si>
+    <t>Macro 1 wrt 9</t>
+  </si>
+  <si>
+    <t>Macro 0 wrt 9</t>
   </si>
 </sst>
 </file>
@@ -542,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,6 +1336,58 @@
         <v>12</v>
       </c>
     </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="3">
+        <v>88.24</v>
+      </c>
+      <c r="H26" s="3">
+        <v>88.09</v>
+      </c>
+      <c r="I26" s="3">
+        <v>87.93</v>
+      </c>
+      <c r="J26" s="3">
+        <v>74.760000000000005</v>
+      </c>
+      <c r="K26" s="3">
+        <v>76.42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Exp 30 htm parameters and output
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9D5C00-D220-400D-876F-BC7084F6CBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D967B65E-8489-46D9-9167-16C249516933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -208,6 +208,24 @@
   </si>
   <si>
     <t>Macro 0 wrt 9</t>
+  </si>
+  <si>
+    <t>Exp 29.png</t>
+  </si>
+  <si>
+    <t>Exp 29</t>
+  </si>
+  <si>
+    <t>Exp 30</t>
+  </si>
+  <si>
+    <t>Exp 30.png</t>
+  </si>
+  <si>
+    <t>Exp 31</t>
+  </si>
+  <si>
+    <t>Exp 31.png</t>
   </si>
 </sst>
 </file>
@@ -557,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,6 +1406,111 @@
         <v>76.42</v>
       </c>
     </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="3">
+        <v>66.319999999999993</v>
+      </c>
+      <c r="H27" s="3">
+        <v>67.150000000000006</v>
+      </c>
+      <c r="I27" s="3">
+        <v>54.64</v>
+      </c>
+      <c r="J27" s="3">
+        <v>48.68</v>
+      </c>
+      <c r="K27" s="3">
+        <v>45.74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="C28" s="3">
+        <v>30</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" s="3">
+        <v>63.38</v>
+      </c>
+      <c r="H28" s="3">
+        <v>62</v>
+      </c>
+      <c r="I28" s="3">
+        <v>79.569999999999993</v>
+      </c>
+      <c r="J28" s="3">
+        <v>45.89</v>
+      </c>
+      <c r="K28" s="3">
+        <v>48.16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C29" s="3">
+        <v>30</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="5">
+        <v>22.19</v>
+      </c>
+      <c r="H29" s="5">
+        <v>17.309999999999999</v>
+      </c>
+      <c r="I29" s="5">
+        <v>53.17</v>
+      </c>
+      <c r="J29" s="5">
+        <v>9.26</v>
+      </c>
+      <c r="K29" s="5">
+        <v>12.43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Conducting Experiments for Different Parameters
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D967B65E-8489-46D9-9167-16C249516933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05769916-18CB-4F40-BF48-4255546CAD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="20460" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="106">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -226,6 +226,123 @@
   </si>
   <si>
     <t>Exp 31.png</t>
+  </si>
+  <si>
+    <t>Exp 32</t>
+  </si>
+  <si>
+    <t>Exp 32.png</t>
+  </si>
+  <si>
+    <t>Exp 34</t>
+  </si>
+  <si>
+    <t>Exp 35</t>
+  </si>
+  <si>
+    <t>Exp 36</t>
+  </si>
+  <si>
+    <t>Exp 35.png</t>
+  </si>
+  <si>
+    <t>Exp 34.png</t>
+  </si>
+  <si>
+    <t>Exp 36.png</t>
+  </si>
+  <si>
+    <t>Exp 37</t>
+  </si>
+  <si>
+    <t>Exp 37.png</t>
+  </si>
+  <si>
+    <t>Exp 38</t>
+  </si>
+  <si>
+    <t>Exp 38.png</t>
+  </si>
+  <si>
+    <t>Exp 39</t>
+  </si>
+  <si>
+    <t>Exp 39.png</t>
+  </si>
+  <si>
+    <t>Exp 40</t>
+  </si>
+  <si>
+    <t>Exp 40.png</t>
+  </si>
+  <si>
+    <t>Exp 41</t>
+  </si>
+  <si>
+    <t>Exp 41.png</t>
+  </si>
+  <si>
+    <t>Exp 42</t>
+  </si>
+  <si>
+    <t>Exp 42.png</t>
+  </si>
+  <si>
+    <t>Exp 43</t>
+  </si>
+  <si>
+    <t>Exp 43.png</t>
+  </si>
+  <si>
+    <t>Exp 44</t>
+  </si>
+  <si>
+    <t>Exp 44.png</t>
+  </si>
+  <si>
+    <t>Exp 45</t>
+  </si>
+  <si>
+    <t>Exp 45.png</t>
+  </si>
+  <si>
+    <t>Exp 46</t>
+  </si>
+  <si>
+    <t>Exp 46.png</t>
+  </si>
+  <si>
+    <t>Exp 47</t>
+  </si>
+  <si>
+    <t>Exp 47.png</t>
+  </si>
+  <si>
+    <t>Exp 48</t>
+  </si>
+  <si>
+    <t>Exp 48.png</t>
+  </si>
+  <si>
+    <t>Exp 49</t>
+  </si>
+  <si>
+    <t>Exp 50</t>
+  </si>
+  <si>
+    <t>Exp 50.png</t>
+  </si>
+  <si>
+    <t>Exp 51</t>
+  </si>
+  <si>
+    <t>Exp 51.png</t>
+  </si>
+  <si>
+    <t>Exp 52</t>
+  </si>
+  <si>
+    <t>Exp 52.png</t>
   </si>
 </sst>
 </file>
@@ -241,7 +358,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +368,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -282,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -295,6 +418,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,10 +1098,10 @@
       <c r="I11" s="5">
         <v>93.24</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="3">
         <v>92.72</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="3">
         <v>94.72</v>
       </c>
     </row>
@@ -1003,7 +1130,7 @@
       <c r="H12" s="5">
         <v>96.52</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="3">
         <v>90.85</v>
       </c>
       <c r="J12" s="5">
@@ -1041,7 +1168,7 @@
       <c r="I13" s="5">
         <v>88.01</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="3">
         <v>88.32</v>
       </c>
       <c r="K13" s="5">
@@ -1210,7 +1337,7 @@
       <c r="G18" s="5">
         <v>87.76</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="3">
         <v>78.650000000000006</v>
       </c>
       <c r="I18" s="5">
@@ -1511,6 +1638,616 @@
         <v>12.43</v>
       </c>
     </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C30" s="3">
+        <v>30</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>68</v>
+      </c>
+      <c r="G30" s="5">
+        <v>82.86</v>
+      </c>
+      <c r="H30" s="5">
+        <v>78.319999999999993</v>
+      </c>
+      <c r="I30" s="5">
+        <v>93.31</v>
+      </c>
+      <c r="J30" s="5">
+        <v>70.94</v>
+      </c>
+      <c r="K30" s="5">
+        <v>77.05</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="C31" s="3">
+        <v>30</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>73</v>
+      </c>
+      <c r="G31" s="5">
+        <v>97.28</v>
+      </c>
+      <c r="H31" s="5">
+        <v>95.44</v>
+      </c>
+      <c r="I31" s="5">
+        <v>99.34</v>
+      </c>
+      <c r="J31" s="5">
+        <v>95.87</v>
+      </c>
+      <c r="K31" s="5">
+        <v>97.01</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="C32" s="3">
+        <v>20</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>72</v>
+      </c>
+      <c r="G32" s="5">
+        <v>97.53</v>
+      </c>
+      <c r="H32" s="5">
+        <v>95.03</v>
+      </c>
+      <c r="I32" s="5">
+        <v>99.4</v>
+      </c>
+      <c r="J32" s="5">
+        <v>95.98</v>
+      </c>
+      <c r="K32" s="5">
+        <v>97.15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C33" s="3">
+        <v>20</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>74</v>
+      </c>
+      <c r="G33" s="5">
+        <v>95.08</v>
+      </c>
+      <c r="H33" s="5">
+        <v>90.96</v>
+      </c>
+      <c r="I33" s="5">
+        <v>98.47</v>
+      </c>
+      <c r="J33" s="5">
+        <v>92.49</v>
+      </c>
+      <c r="K33" s="5">
+        <v>93.95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="C34" s="3">
+        <v>20</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>76</v>
+      </c>
+      <c r="G34" s="5">
+        <v>91.69</v>
+      </c>
+      <c r="H34" s="5">
+        <v>86.11</v>
+      </c>
+      <c r="I34" s="5">
+        <v>97.2</v>
+      </c>
+      <c r="J34" s="5">
+        <v>88.07</v>
+      </c>
+      <c r="K34" s="5">
+        <v>89.39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="C35" s="3">
+        <v>20</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>78</v>
+      </c>
+      <c r="G35" s="5">
+        <v>88.97</v>
+      </c>
+      <c r="H35" s="5">
+        <v>82.83</v>
+      </c>
+      <c r="I35" s="5">
+        <v>95.64</v>
+      </c>
+      <c r="J35" s="5">
+        <v>81.849999999999994</v>
+      </c>
+      <c r="K35" s="5">
+        <v>84.17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C36" s="3">
+        <v>20</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>80</v>
+      </c>
+      <c r="G36" s="5">
+        <v>83.78</v>
+      </c>
+      <c r="H36" s="5">
+        <v>78.66</v>
+      </c>
+      <c r="I36" s="5">
+        <v>92.67</v>
+      </c>
+      <c r="J36" s="5">
+        <v>71.819999999999993</v>
+      </c>
+      <c r="K36" s="5">
+        <v>76.459999999999994</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="C37" s="3">
+        <v>20</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>82</v>
+      </c>
+      <c r="G37" s="5">
+        <v>74.78</v>
+      </c>
+      <c r="H37" s="5">
+        <v>73.8</v>
+      </c>
+      <c r="I37" s="5">
+        <v>87.3</v>
+      </c>
+      <c r="J37" s="5">
+        <v>59.76</v>
+      </c>
+      <c r="K37" s="5">
+        <v>62.82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="C38" s="3">
+        <v>20</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>84</v>
+      </c>
+      <c r="G38" s="5">
+        <v>64.36</v>
+      </c>
+      <c r="H38" s="5">
+        <v>64.11</v>
+      </c>
+      <c r="I38" s="5">
+        <v>77.459999999999994</v>
+      </c>
+      <c r="J38" s="5">
+        <v>44.26</v>
+      </c>
+      <c r="K38" s="5">
+        <v>50.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C39" s="3">
+        <v>20</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F39" t="s">
+        <v>86</v>
+      </c>
+      <c r="G39" s="5">
+        <v>60.54</v>
+      </c>
+      <c r="H39" s="5">
+        <v>57.42</v>
+      </c>
+      <c r="I39" s="5">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="J39" s="5">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="K39" s="5">
+        <v>35.54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="C40" s="3">
+        <v>20</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>88</v>
+      </c>
+      <c r="G40" s="5">
+        <v>33.71</v>
+      </c>
+      <c r="H40" s="5">
+        <v>39.08</v>
+      </c>
+      <c r="I40" s="5">
+        <v>38.270000000000003</v>
+      </c>
+      <c r="J40" s="5">
+        <v>16.440000000000001</v>
+      </c>
+      <c r="K40" s="5">
+        <v>44.29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C41" s="3">
+        <v>10</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>90</v>
+      </c>
+      <c r="G41" s="5">
+        <v>20.2</v>
+      </c>
+      <c r="H41" s="5">
+        <v>26.74</v>
+      </c>
+      <c r="I41" s="5">
+        <v>24.88</v>
+      </c>
+      <c r="J41" s="5">
+        <v>17.739999999999998</v>
+      </c>
+      <c r="K41" s="5">
+        <v>22.44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C42" s="3">
+        <v>10</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>92</v>
+      </c>
+      <c r="G42" s="5">
+        <v>56.03</v>
+      </c>
+      <c r="H42" s="5">
+        <v>58.29</v>
+      </c>
+      <c r="I42" s="5">
+        <v>56.72</v>
+      </c>
+      <c r="J42" s="5">
+        <v>40.32</v>
+      </c>
+      <c r="K42" s="5">
+        <v>59.71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="C43" s="3">
+        <v>10</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="C44" s="6">
+        <v>10</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="6">
+        <v>-1</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G44" s="7">
+        <v>79.59</v>
+      </c>
+      <c r="H44" s="7">
+        <v>76.78</v>
+      </c>
+      <c r="I44" s="7">
+        <v>74.53</v>
+      </c>
+      <c r="J44" s="7">
+        <v>57.48</v>
+      </c>
+      <c r="K44" s="7">
+        <v>55.46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="C45" s="3">
+        <v>10</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="C46" s="3">
+        <v>10</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F46" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="C47" s="3">
+        <v>10</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="C48" s="3">
+        <v>10</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B49" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C49" s="3">
+        <v>10</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F49" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Working on Label Prediction
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05769916-18CB-4F40-BF48-4255546CAD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F40E8F-7C0D-4715-B7C6-9A440955B957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="15" windowWidth="20460" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="107">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>Exp 52.png</t>
+  </si>
+  <si>
+    <t>Exp 53</t>
   </si>
 </sst>
 </file>
@@ -702,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2248,6 +2251,23 @@
         <v>105</v>
       </c>
     </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C50" s="3">
+        <v>10</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" s="3">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating Analysis in Excel
</commit_message>
<xml_diff>
--- a/My Analysis/Changes In HTM Parameters.xlsx
+++ b/My Analysis/Changes In HTM Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\neocortexapi-classification\My Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBC56CF-FDE6-4604-A2FE-66D5D813B8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2808DD70-46CA-45B6-AC06-6A6CBD789564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="164">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -480,6 +480,46 @@
   </si>
   <si>
     <t>Exp 75.png</t>
+  </si>
+  <si>
+    <t>No Overlapping between Min. of Micro and Max. of Macro</t>
+  </si>
+  <si>
+    <t>Some Overlapping</t>
+  </si>
+  <si>
+    <t>Some Overlapping (Similarity too low)</t>
+  </si>
+  <si>
+    <t>Overlapping</t>
+  </si>
+  <si>
+    <t>Exp 33</t>
+  </si>
+  <si>
+    <t>Exp 33.png</t>
+  </si>
+  <si>
+    <t>Overlapping (Similarity too high)</t>
+  </si>
+  <si>
+    <t>Overlapping (Cross correlation too high)</t>
+  </si>
+  <si>
+    <t>100% Overlapping</t>
+  </si>
+  <si>
+    <t>No Overlapping between Min. of Micro and Max. of Macro,
+but cross correlation too high</t>
+  </si>
+  <si>
+    <t>Some Overlapping, cross correlation too high</t>
+  </si>
+  <si>
+    <t>Some Overlapping,</t>
+  </si>
+  <si>
+    <t>Very Small Overlapping</t>
   </si>
 </sst>
 </file>
@@ -501,7 +541,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -520,8 +560,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -544,11 +596,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -564,10 +642,31 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2071,25 +2170,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L71"/>
+  <dimension ref="A1:M72"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25:K71"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C55" sqref="C48:I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="3" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" customWidth="1"/>
     <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="52.28515625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2105,7 +2205,7 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -2120,11 +2220,12 @@
       <c r="J1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="12" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M1" s="13"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -2140,7 +2241,7 @@
       <c r="E2" s="3">
         <v>-1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="3">
@@ -2159,7 +2260,7 @@
         <v>72.06</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -2175,7 +2276,7 @@
       <c r="E3" s="3">
         <v>-1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="3">
@@ -2194,7 +2295,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -2210,7 +2311,7 @@
       <c r="E4" s="3">
         <v>-1</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="3">
@@ -2229,7 +2330,7 @@
         <v>99.65</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -2245,7 +2346,7 @@
       <c r="E5" s="3">
         <v>-1</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="5">
@@ -2264,7 +2365,7 @@
         <v>99.22</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -2280,7 +2381,7 @@
       <c r="E6" s="3">
         <v>-1</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G6" s="5">
@@ -2299,7 +2400,7 @@
         <v>98.56</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -2315,7 +2416,7 @@
       <c r="E7" s="3">
         <v>-1</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G7" s="5">
@@ -2334,7 +2435,7 @@
         <v>97.87</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -2350,7 +2451,7 @@
       <c r="E8" s="3">
         <v>-1</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="5">
@@ -2369,7 +2470,7 @@
         <v>96.99</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
@@ -2385,7 +2486,7 @@
       <c r="E9" s="3">
         <v>-1</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="3" t="s">
         <v>24</v>
       </c>
       <c r="G9" s="5">
@@ -2404,7 +2505,7 @@
         <v>96.22</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
@@ -2420,7 +2521,7 @@
       <c r="E10" s="3">
         <v>-1</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="3" t="s">
         <v>26</v>
       </c>
       <c r="G10" s="5">
@@ -2439,7 +2540,7 @@
         <v>95.51</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
@@ -2455,7 +2556,7 @@
       <c r="E11" s="3">
         <v>-1</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="3" t="s">
         <v>28</v>
       </c>
       <c r="G11" s="5">
@@ -2474,7 +2575,7 @@
         <v>94.72</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
@@ -2490,7 +2591,7 @@
       <c r="E12" s="3">
         <v>-1</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="G12" s="5">
@@ -2509,7 +2610,7 @@
         <v>93.68</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
@@ -2525,7 +2626,7 @@
       <c r="E13" s="3">
         <v>-1</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G13" s="5">
@@ -2544,7 +2645,7 @@
         <v>91.62</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
@@ -2560,7 +2661,7 @@
       <c r="E14" s="3">
         <v>-1</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G14" s="5">
@@ -2579,7 +2680,7 @@
         <v>88.79</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>35</v>
       </c>
@@ -2595,7 +2696,7 @@
       <c r="E15" s="3">
         <v>-1</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="3" t="s">
         <v>36</v>
       </c>
       <c r="G15" s="5">
@@ -2614,7 +2715,7 @@
         <v>85.63</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>37</v>
       </c>
@@ -2630,7 +2731,7 @@
       <c r="E16" s="3">
         <v>-1</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="3" t="s">
         <v>38</v>
       </c>
       <c r="G16" s="5">
@@ -2649,7 +2750,7 @@
         <v>84.47</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>39</v>
       </c>
@@ -2665,7 +2766,7 @@
       <c r="E17" s="3">
         <v>-1</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G17" s="5">
@@ -2684,7 +2785,7 @@
         <v>79.63</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
@@ -2700,7 +2801,7 @@
       <c r="E18" s="3">
         <v>-1</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G18" s="5">
@@ -2719,7 +2820,7 @@
         <v>87.76</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>44</v>
       </c>
@@ -2735,7 +2836,7 @@
       <c r="E19" s="3">
         <v>-1</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G19" s="5">
@@ -2754,7 +2855,7 @@
         <v>85.34</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>45</v>
       </c>
@@ -2770,7 +2871,7 @@
       <c r="E20" s="3">
         <v>-1</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="3" t="s">
         <v>46</v>
       </c>
       <c r="G20" s="5">
@@ -2789,8 +2890,11 @@
         <v>81.59</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="7"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>47</v>
       </c>
@@ -2806,11 +2910,11 @@
       <c r="E22" s="3">
         <v>-1</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>48</v>
       </c>
@@ -2826,11 +2930,11 @@
       <c r="E23" s="3">
         <v>-1</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>11</v>
       </c>
@@ -2846,11 +2950,11 @@
       <c r="E24" s="3">
         <v>-1</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G25" s="1" t="s">
         <v>58</v>
       </c>
@@ -2863,11 +2967,11 @@
       <c r="J25" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="K25" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>56</v>
       </c>
@@ -2883,26 +2987,29 @@
       <c r="E26" s="3">
         <v>-1</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="8">
         <v>88.24</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="8">
         <v>88.09</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26" s="8">
         <v>87.93</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="8">
         <v>74.760000000000005</v>
       </c>
-      <c r="K26" s="3">
+      <c r="K26" s="8">
         <v>76.42</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>62</v>
       </c>
@@ -2918,7 +3025,7 @@
       <c r="E27" s="3">
         <v>-1</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="3" t="s">
         <v>61</v>
       </c>
       <c r="G27" s="3">
@@ -2936,8 +3043,11 @@
       <c r="K27" s="3">
         <v>45.74</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>63</v>
       </c>
@@ -2953,7 +3063,7 @@
       <c r="E28" s="3">
         <v>-1</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="3" t="s">
         <v>64</v>
       </c>
       <c r="G28" s="3">
@@ -2971,8 +3081,11 @@
       <c r="K28" s="3">
         <v>48.16</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>65</v>
       </c>
@@ -2988,7 +3101,7 @@
       <c r="E29" s="3">
         <v>-1</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="3" t="s">
         <v>66</v>
       </c>
       <c r="G29" s="5">
@@ -3006,8 +3119,11 @@
       <c r="K29" s="5">
         <v>12.43</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>67</v>
       </c>
@@ -3023,7 +3139,7 @@
       <c r="E30" s="3">
         <v>-1</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="3" t="s">
         <v>68</v>
       </c>
       <c r="G30" s="5">
@@ -3041,10 +3157,13 @@
       <c r="K30" s="5">
         <v>77.05</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" s="14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>69</v>
+        <v>155</v>
       </c>
       <c r="B31" s="3">
         <v>0.7</v>
@@ -3058,34 +3177,37 @@
       <c r="E31" s="3">
         <v>-1</v>
       </c>
-      <c r="F31" t="s">
-        <v>73</v>
+      <c r="F31" s="3" t="s">
+        <v>156</v>
       </c>
       <c r="G31" s="5">
-        <v>97.28</v>
+        <v>91.87</v>
       </c>
       <c r="H31" s="5">
-        <v>95.44</v>
+        <v>85.52</v>
       </c>
       <c r="I31" s="5">
-        <v>99.34</v>
+        <v>97.1</v>
       </c>
       <c r="J31" s="5">
-        <v>95.87</v>
+        <v>86.95</v>
       </c>
       <c r="K31" s="5">
-        <v>97.01</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>90.65</v>
+      </c>
+      <c r="L31" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B32" s="3">
         <v>0.9</v>
       </c>
       <c r="C32" s="3">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>4</v>
@@ -3093,31 +3215,34 @@
       <c r="E32" s="3">
         <v>-1</v>
       </c>
-      <c r="F32" t="s">
-        <v>72</v>
+      <c r="F32" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="G32" s="5">
-        <v>97.53</v>
+        <v>97.28</v>
       </c>
       <c r="H32" s="5">
-        <v>95.03</v>
+        <v>95.44</v>
       </c>
       <c r="I32" s="5">
-        <v>99.4</v>
+        <v>99.34</v>
       </c>
       <c r="J32" s="5">
-        <v>95.98</v>
+        <v>95.87</v>
       </c>
       <c r="K32" s="5">
-        <v>97.15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>97.01</v>
+      </c>
+      <c r="L32" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B33" s="3">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="C33" s="3">
         <v>20</v>
@@ -3128,31 +3253,34 @@
       <c r="E33" s="3">
         <v>-1</v>
       </c>
-      <c r="F33" t="s">
-        <v>74</v>
+      <c r="F33" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="G33" s="5">
-        <v>95.08</v>
+        <v>97.53</v>
       </c>
       <c r="H33" s="5">
-        <v>90.96</v>
+        <v>95.03</v>
       </c>
       <c r="I33" s="5">
-        <v>98.47</v>
+        <v>99.4</v>
       </c>
       <c r="J33" s="5">
-        <v>92.49</v>
+        <v>95.98</v>
       </c>
       <c r="K33" s="5">
-        <v>93.95</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>97.15</v>
+      </c>
+      <c r="L33" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B34" s="3">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="C34" s="3">
         <v>20</v>
@@ -3163,31 +3291,34 @@
       <c r="E34" s="3">
         <v>-1</v>
       </c>
-      <c r="F34" t="s">
-        <v>76</v>
+      <c r="F34" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="G34" s="5">
-        <v>91.69</v>
+        <v>95.05</v>
       </c>
       <c r="H34" s="5">
-        <v>86.11</v>
+        <v>91.05</v>
       </c>
       <c r="I34" s="5">
-        <v>97.2</v>
+        <v>98.47</v>
       </c>
       <c r="J34" s="5">
-        <v>88.07</v>
+        <v>92.4</v>
       </c>
       <c r="K34" s="5">
-        <v>89.39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+        <v>93.74</v>
+      </c>
+      <c r="L34" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B35" s="3">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="C35" s="3">
         <v>20</v>
@@ -3198,31 +3329,34 @@
       <c r="E35" s="3">
         <v>-1</v>
       </c>
-      <c r="F35" t="s">
-        <v>78</v>
+      <c r="F35" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="G35" s="5">
-        <v>88.97</v>
+        <v>91.69</v>
       </c>
       <c r="H35" s="5">
-        <v>82.83</v>
+        <v>86.11</v>
       </c>
       <c r="I35" s="5">
-        <v>95.64</v>
+        <v>97.2</v>
       </c>
       <c r="J35" s="5">
-        <v>81.849999999999994</v>
+        <v>88.07</v>
       </c>
       <c r="K35" s="5">
-        <v>84.17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>89.39</v>
+      </c>
+      <c r="L35" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B36" s="3">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="C36" s="3">
         <v>20</v>
@@ -3233,31 +3367,34 @@
       <c r="E36" s="3">
         <v>-1</v>
       </c>
-      <c r="F36" t="s">
-        <v>80</v>
+      <c r="F36" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="G36" s="5">
-        <v>83.78</v>
+        <v>88.97</v>
       </c>
       <c r="H36" s="5">
-        <v>78.66</v>
+        <v>82.83</v>
       </c>
       <c r="I36" s="5">
-        <v>92.67</v>
+        <v>95.64</v>
       </c>
       <c r="J36" s="5">
-        <v>71.819999999999993</v>
+        <v>81.849999999999994</v>
       </c>
       <c r="K36" s="5">
-        <v>76.459999999999994</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+        <v>84.17</v>
+      </c>
+      <c r="L36" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B37" s="3">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="C37" s="3">
         <v>20</v>
@@ -3268,31 +3405,34 @@
       <c r="E37" s="3">
         <v>-1</v>
       </c>
-      <c r="F37" t="s">
-        <v>82</v>
+      <c r="F37" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="G37" s="5">
-        <v>74.78</v>
+        <v>83.78</v>
       </c>
       <c r="H37" s="5">
-        <v>73.8</v>
+        <v>78.66</v>
       </c>
       <c r="I37" s="5">
-        <v>87.3</v>
+        <v>92.67</v>
       </c>
       <c r="J37" s="5">
-        <v>59.76</v>
+        <v>71.819999999999993</v>
       </c>
       <c r="K37" s="5">
-        <v>62.82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>76.459999999999994</v>
+      </c>
+      <c r="L37" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B38" s="3">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="C38" s="3">
         <v>20</v>
@@ -3303,31 +3443,34 @@
       <c r="E38" s="3">
         <v>-1</v>
       </c>
-      <c r="F38" t="s">
-        <v>84</v>
+      <c r="F38" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="G38" s="5">
-        <v>64.36</v>
+        <v>74.78</v>
       </c>
       <c r="H38" s="5">
-        <v>64.11</v>
+        <v>73.8</v>
       </c>
       <c r="I38" s="5">
-        <v>77.459999999999994</v>
+        <v>87.3</v>
       </c>
       <c r="J38" s="5">
-        <v>44.26</v>
+        <v>59.76</v>
       </c>
       <c r="K38" s="5">
-        <v>50.2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>62.82</v>
+      </c>
+      <c r="L38" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B39" s="3">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="C39" s="3">
         <v>20</v>
@@ -3338,31 +3481,34 @@
       <c r="E39" s="3">
         <v>-1</v>
       </c>
-      <c r="F39" t="s">
-        <v>86</v>
+      <c r="F39" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="G39" s="5">
-        <v>60.54</v>
+        <v>64.36</v>
       </c>
       <c r="H39" s="5">
-        <v>57.42</v>
+        <v>64.11</v>
       </c>
       <c r="I39" s="5">
-        <v>74.900000000000006</v>
+        <v>77.459999999999994</v>
       </c>
       <c r="J39" s="5">
-        <v>37.299999999999997</v>
+        <v>44.26</v>
       </c>
       <c r="K39" s="5">
-        <v>35.54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+        <v>50.2</v>
+      </c>
+      <c r="L39" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B40" s="3">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="C40" s="3">
         <v>20</v>
@@ -3373,66 +3519,72 @@
       <c r="E40" s="3">
         <v>-1</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G40" s="5">
+        <v>60.54</v>
+      </c>
+      <c r="H40" s="5">
+        <v>57.42</v>
+      </c>
+      <c r="I40" s="5">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="J40" s="5">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="K40" s="5">
+        <v>35.54</v>
+      </c>
+      <c r="L40" s="14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="C41" s="3">
+        <v>20</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G41" s="5">
         <v>33.71</v>
       </c>
-      <c r="H40" s="5">
+      <c r="H41" s="5">
         <v>39.08</v>
       </c>
-      <c r="I40" s="5">
+      <c r="I41" s="5">
         <v>38.270000000000003</v>
       </c>
-      <c r="J40" s="5">
+      <c r="J41" s="5">
         <v>16.440000000000001</v>
       </c>
-      <c r="K40" s="5">
+      <c r="K41" s="5">
         <v>44.29</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="L41" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B42" s="3">
         <v>0.1</v>
-      </c>
-      <c r="C41" s="3">
-        <v>10</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E41" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F41" t="s">
-        <v>90</v>
-      </c>
-      <c r="G41" s="5">
-        <v>20.2</v>
-      </c>
-      <c r="H41" s="5">
-        <v>26.74</v>
-      </c>
-      <c r="I41" s="5">
-        <v>24.88</v>
-      </c>
-      <c r="J41" s="5">
-        <v>17.739999999999998</v>
-      </c>
-      <c r="K41" s="5">
-        <v>22.44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B42" s="3">
-        <v>0.2</v>
       </c>
       <c r="C42" s="3">
         <v>10</v>
@@ -3443,101 +3595,110 @@
       <c r="E42" s="3">
         <v>-1</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G42" s="5">
+        <v>20.2</v>
+      </c>
+      <c r="H42" s="5">
+        <v>26.74</v>
+      </c>
+      <c r="I42" s="5">
+        <v>24.88</v>
+      </c>
+      <c r="J42" s="5">
+        <v>17.739999999999998</v>
+      </c>
+      <c r="K42" s="5">
+        <v>22.44</v>
+      </c>
+      <c r="L42" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C43" s="3">
+        <v>10</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="G42" s="5">
+      <c r="G43" s="5">
         <v>56.03</v>
       </c>
-      <c r="H42" s="5">
+      <c r="H43" s="5">
         <v>58.29</v>
       </c>
-      <c r="I42" s="5">
+      <c r="I43" s="5">
         <v>56.72</v>
       </c>
-      <c r="J42" s="5">
+      <c r="J43" s="5">
         <v>40.32</v>
       </c>
-      <c r="K42" s="5">
+      <c r="K43" s="5">
         <v>59.71</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+      <c r="L43" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B44" s="8">
         <v>0.3</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C44" s="8">
         <v>10</v>
       </c>
-      <c r="D43" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E43" s="6">
-        <v>-1</v>
-      </c>
-      <c r="F43" s="7" t="s">
+      <c r="D44" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="8">
+        <v>-1</v>
+      </c>
+      <c r="F44" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="G43" s="6">
+      <c r="G44" s="8">
         <v>79.59</v>
       </c>
-      <c r="H43" s="6">
+      <c r="H44" s="8">
         <v>76.78</v>
       </c>
-      <c r="I43" s="6">
+      <c r="I44" s="8">
         <v>74.53</v>
       </c>
-      <c r="J43" s="6">
+      <c r="J44" s="8">
         <v>57.48</v>
       </c>
-      <c r="K43" s="6">
+      <c r="K44" s="8">
         <v>55.46</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="L44" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B45" s="3">
         <v>0.35</v>
-      </c>
-      <c r="C44" s="3">
-        <v>10</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E44" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F44" t="s">
-        <v>96</v>
-      </c>
-      <c r="G44" s="5">
-        <v>86.3</v>
-      </c>
-      <c r="H44" s="5">
-        <v>79.63</v>
-      </c>
-      <c r="I44" s="5">
-        <v>80.150000000000006</v>
-      </c>
-      <c r="J44" s="5">
-        <v>60.43</v>
-      </c>
-      <c r="K44" s="5">
-        <v>54.91</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B45" s="3">
-        <v>0.38</v>
       </c>
       <c r="C45" s="3">
         <v>10</v>
@@ -3548,31 +3709,34 @@
       <c r="E45" s="3">
         <v>-1</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="G45" s="3">
-        <v>86.77</v>
-      </c>
-      <c r="H45" s="3">
-        <v>80.48</v>
-      </c>
-      <c r="I45" s="3">
-        <v>82.88</v>
-      </c>
-      <c r="J45" s="3">
-        <v>63.5</v>
-      </c>
-      <c r="K45" s="3">
-        <v>55.1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G45" s="5">
+        <v>86.3</v>
+      </c>
+      <c r="H45" s="5">
+        <v>79.63</v>
+      </c>
+      <c r="I45" s="5">
+        <v>80.150000000000006</v>
+      </c>
+      <c r="J45" s="5">
+        <v>60.43</v>
+      </c>
+      <c r="K45" s="5">
+        <v>54.91</v>
+      </c>
+      <c r="L45" s="16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B46" s="3">
-        <v>0.4</v>
+        <v>0.38</v>
       </c>
       <c r="C46" s="3">
         <v>10</v>
@@ -3583,101 +3747,110 @@
       <c r="E46" s="3">
         <v>-1</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G46" s="3">
+        <v>86.77</v>
+      </c>
+      <c r="H46" s="3">
+        <v>80.48</v>
+      </c>
+      <c r="I46" s="3">
+        <v>82.88</v>
+      </c>
+      <c r="J46" s="3">
+        <v>63.5</v>
+      </c>
+      <c r="K46" s="3">
+        <v>55.1</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="C47" s="8">
+        <v>10</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="8">
+        <v>-1</v>
+      </c>
+      <c r="F47" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="G46" s="3">
+      <c r="G47" s="8">
         <v>85.8</v>
       </c>
-      <c r="H46" s="3">
+      <c r="H47" s="8">
         <v>82.57</v>
       </c>
-      <c r="I46" s="3">
+      <c r="I47" s="8">
         <v>84.52</v>
       </c>
-      <c r="J46" s="3">
+      <c r="J47" s="8">
         <v>66.819999999999993</v>
       </c>
-      <c r="K46" s="3">
+      <c r="K47" s="8">
         <v>56.35</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="L47" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B48" s="8">
         <v>0.45</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C48" s="8">
         <v>10</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E47" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F47" t="s">
+      <c r="D48" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" s="8">
+        <v>-1</v>
+      </c>
+      <c r="F48" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G48" s="8">
         <v>85.23</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H48" s="8">
         <v>84.88</v>
       </c>
-      <c r="I47" s="3">
+      <c r="I48" s="8">
         <v>85.15</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J48" s="8">
         <v>71.94</v>
       </c>
-      <c r="K47" s="3">
+      <c r="K48" s="8">
         <v>58.86</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="L48" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B49" s="3">
         <v>0.5</v>
-      </c>
-      <c r="C48" s="3">
-        <v>10</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E48" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F48" t="s">
-        <v>103</v>
-      </c>
-      <c r="G48" s="3">
-        <v>89.11</v>
-      </c>
-      <c r="H48" s="3">
-        <v>85.44</v>
-      </c>
-      <c r="I48" s="3">
-        <v>88.15</v>
-      </c>
-      <c r="J48" s="3">
-        <v>77.47</v>
-      </c>
-      <c r="K48" s="3">
-        <v>64.430000000000007</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B49" s="3">
-        <v>0.55000000000000004</v>
       </c>
       <c r="C49" s="3">
         <v>10</v>
@@ -3688,31 +3861,34 @@
       <c r="E49" s="3">
         <v>-1</v>
       </c>
-      <c r="F49" t="s">
-        <v>111</v>
+      <c r="F49" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="G49" s="3">
-        <v>90.06</v>
+        <v>89.11</v>
       </c>
       <c r="H49" s="3">
-        <v>88.23</v>
+        <v>85.44</v>
       </c>
       <c r="I49" s="3">
-        <v>90.75</v>
+        <v>88.15</v>
       </c>
       <c r="J49" s="3">
-        <v>79.23</v>
+        <v>77.47</v>
       </c>
       <c r="K49" s="3">
-        <v>68.48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+        <v>64.430000000000007</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B50" s="3">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C50" s="3">
         <v>10</v>
@@ -3723,31 +3899,34 @@
       <c r="E50" s="3">
         <v>-1</v>
       </c>
-      <c r="F50" t="s">
-        <v>110</v>
+      <c r="F50" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="G50" s="3">
-        <v>92.7</v>
+        <v>90.06</v>
       </c>
       <c r="H50" s="3">
-        <v>89.98</v>
+        <v>88.23</v>
       </c>
       <c r="I50" s="3">
-        <v>93.3</v>
+        <v>90.75</v>
       </c>
       <c r="J50" s="3">
-        <v>82.22</v>
+        <v>79.23</v>
       </c>
       <c r="K50" s="3">
-        <v>74.39</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+        <v>68.48</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B51" s="3">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="C51" s="3">
         <v>10</v>
@@ -3758,31 +3937,34 @@
       <c r="E51" s="3">
         <v>-1</v>
       </c>
-      <c r="F51" t="s">
-        <v>109</v>
+      <c r="F51" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="G51" s="3">
-        <v>93.9</v>
+        <v>92.7</v>
       </c>
       <c r="H51" s="3">
-        <v>91.87</v>
+        <v>89.98</v>
       </c>
       <c r="I51" s="3">
-        <v>94.22</v>
+        <v>93.3</v>
       </c>
       <c r="J51" s="3">
-        <v>86.46</v>
+        <v>82.22</v>
       </c>
       <c r="K51" s="3">
-        <v>79.239999999999995</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+        <v>74.39</v>
+      </c>
+      <c r="L51" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B52" s="3">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="C52" s="3">
         <v>10</v>
@@ -3793,31 +3975,34 @@
       <c r="E52" s="3">
         <v>-1</v>
       </c>
-      <c r="F52" t="s">
-        <v>108</v>
+      <c r="F52" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="G52" s="3">
-        <v>94.04</v>
+        <v>93.9</v>
       </c>
       <c r="H52" s="3">
-        <v>94.97</v>
+        <v>91.87</v>
       </c>
       <c r="I52" s="3">
-        <v>94.91</v>
+        <v>94.22</v>
       </c>
       <c r="J52" s="3">
-        <v>89.67</v>
+        <v>86.46</v>
       </c>
       <c r="K52" s="3">
-        <v>83.43</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+        <v>79.239999999999995</v>
+      </c>
+      <c r="L52" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B53" s="3">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="C53" s="3">
         <v>10</v>
@@ -3828,31 +4013,34 @@
       <c r="E53" s="3">
         <v>-1</v>
       </c>
-      <c r="F53" t="s">
-        <v>128</v>
+      <c r="F53" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="G53" s="3">
-        <v>96.21</v>
+        <v>94.04</v>
       </c>
       <c r="H53" s="3">
-        <v>98.74</v>
+        <v>94.97</v>
       </c>
       <c r="I53" s="3">
-        <v>97.68</v>
+        <v>94.91</v>
       </c>
       <c r="J53" s="3">
-        <v>92.25</v>
+        <v>89.67</v>
       </c>
       <c r="K53" s="3">
-        <v>88.84</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+        <v>83.43</v>
+      </c>
+      <c r="L53" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B54" s="3">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="C54" s="3">
         <v>10</v>
@@ -3863,629 +4051,719 @@
       <c r="E54" s="3">
         <v>-1</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G54" s="3">
+        <v>96.21</v>
+      </c>
+      <c r="H54" s="3">
+        <v>98.74</v>
+      </c>
+      <c r="I54" s="3">
+        <v>97.68</v>
+      </c>
+      <c r="J54" s="3">
+        <v>92.25</v>
+      </c>
+      <c r="K54" s="3">
+        <v>88.84</v>
+      </c>
+      <c r="L54" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B55" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="C55" s="3">
+        <v>10</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F55" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G54" s="3">
+      <c r="G55" s="3">
         <v>99.01</v>
       </c>
-      <c r="H54" s="3">
+      <c r="H55" s="3">
         <v>97.15</v>
       </c>
-      <c r="I54" s="3">
+      <c r="I55" s="3">
         <v>99.24</v>
       </c>
-      <c r="J54" s="3">
+      <c r="J55" s="3">
         <v>94.26</v>
       </c>
-      <c r="K54" s="3">
+      <c r="K55" s="3">
         <v>94.58</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="L55" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B56" s="3">
         <v>0.15</v>
       </c>
-      <c r="C55" s="3">
-        <v>1</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E55" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F55" t="s">
+      <c r="C56" s="3">
+        <v>1</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F56" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="G55" s="3">
+      <c r="G56" s="3">
         <v>68.13</v>
       </c>
-      <c r="H55" s="3">
+      <c r="H56" s="3">
         <v>72.98</v>
       </c>
-      <c r="I55" s="3">
+      <c r="I56" s="3">
         <v>66.459999999999994</v>
       </c>
-      <c r="J55" s="3">
+      <c r="J56" s="3">
         <v>54.61</v>
       </c>
-      <c r="K55" s="3">
+      <c r="K56" s="3">
         <v>56.69</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+      <c r="L56" s="16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B57" s="3">
         <v>0.2</v>
       </c>
-      <c r="C56" s="3">
-        <v>1</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E56" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F56" t="s">
+      <c r="C57" s="3">
+        <v>1</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G56" s="3">
+      <c r="G57" s="3">
         <v>75.95</v>
       </c>
-      <c r="H56" s="3">
+      <c r="H57" s="3">
         <v>78.48</v>
       </c>
-      <c r="I56" s="3">
+      <c r="I57" s="3">
         <v>76.86</v>
       </c>
-      <c r="J56" s="3">
+      <c r="J57" s="3">
         <v>58.9</v>
       </c>
-      <c r="K56" s="3">
+      <c r="K57" s="3">
         <v>57.94</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="L57" s="17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B58" s="3">
         <v>0.25</v>
       </c>
-      <c r="C57" s="3">
-        <v>1</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E57" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F57" t="s">
+      <c r="C58" s="3">
+        <v>1</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E58" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F58" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G57" s="3">
+      <c r="G58" s="3">
         <v>82.92</v>
       </c>
-      <c r="H57" s="3">
+      <c r="H58" s="3">
         <v>79.92</v>
       </c>
-      <c r="I57" s="3">
+      <c r="I58" s="3">
         <v>78.09</v>
       </c>
-      <c r="J57" s="3">
+      <c r="J58" s="3">
         <v>58.8</v>
       </c>
-      <c r="K57" s="3">
+      <c r="K58" s="3">
         <v>65.739999999999995</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="L58" s="16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B58" s="3">
+      <c r="B59" s="3">
         <v>0.3</v>
       </c>
-      <c r="C58" s="3">
-        <v>1</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E58" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F58" t="s">
+      <c r="C59" s="3">
+        <v>1</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E59" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F59" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="G58" s="3">
+      <c r="G59" s="3">
         <v>83.5</v>
       </c>
-      <c r="H58" s="3">
+      <c r="H59" s="3">
         <v>83.1</v>
       </c>
-      <c r="I58" s="3">
+      <c r="I59" s="3">
         <v>82.05</v>
       </c>
-      <c r="J58" s="3">
+      <c r="J59" s="3">
         <v>66.87</v>
       </c>
-      <c r="K58" s="3">
+      <c r="K59" s="3">
         <v>69.19</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="L59" s="15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B60" s="3">
         <v>0.35</v>
       </c>
-      <c r="C59" s="3">
-        <v>1</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E59" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F59" t="s">
+      <c r="C60" s="3">
+        <v>1</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F60" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G59" s="3">
+      <c r="G60" s="3">
         <v>84.19</v>
       </c>
-      <c r="H59" s="3">
+      <c r="H60" s="3">
         <v>87.35</v>
       </c>
-      <c r="I59" s="3">
+      <c r="I60" s="3">
         <v>85.26</v>
       </c>
-      <c r="J59" s="3">
+      <c r="J60" s="3">
         <v>71.92</v>
       </c>
-      <c r="K59" s="3">
+      <c r="K60" s="3">
         <v>73.400000000000006</v>
       </c>
-      <c r="L59" t="s">
+      <c r="L60" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="C61" s="7">
+        <v>1</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G61" s="3">
+        <v>86.64</v>
+      </c>
+      <c r="H61" s="3">
+        <v>87.24</v>
+      </c>
+      <c r="I61" s="3">
+        <v>89.07</v>
+      </c>
+      <c r="J61" s="3">
+        <v>75.64</v>
+      </c>
+      <c r="K61" s="3">
+        <v>77.55</v>
+      </c>
+      <c r="L61" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="M61" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B60" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="C60" s="8">
-        <v>1</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E60" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F60" t="s">
-        <v>135</v>
-      </c>
-      <c r="G60" s="3">
-        <v>86.64</v>
-      </c>
-      <c r="H60" s="3">
-        <v>87.24</v>
-      </c>
-      <c r="I60" s="3">
-        <v>89.07</v>
-      </c>
-      <c r="J60" s="3">
-        <v>75.64</v>
-      </c>
-      <c r="K60" s="3">
-        <v>77.55</v>
-      </c>
-      <c r="L60" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+    <row r="62" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B61" s="3">
+      <c r="B62" s="3">
         <v>0.45</v>
       </c>
-      <c r="C61" s="3">
-        <v>1</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E61" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F61" t="s">
+      <c r="C62" s="3">
+        <v>1</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F62" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G61" s="3">
+      <c r="G62" s="3">
         <v>90.35</v>
       </c>
-      <c r="H61" s="3">
+      <c r="H62" s="3">
         <v>90.72</v>
       </c>
-      <c r="I61" s="3">
+      <c r="I62" s="3">
         <v>91.08</v>
       </c>
-      <c r="J61" s="3">
+      <c r="J62" s="3">
         <v>81.849999999999994</v>
       </c>
-      <c r="K61" s="3">
+      <c r="K62" s="3">
         <v>80.44</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+      <c r="L62" s="18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B62" s="3">
+      <c r="B63" s="3">
         <v>0.5</v>
       </c>
-      <c r="C62" s="3">
-        <v>1</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E62" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F62" t="s">
+      <c r="C63" s="3">
+        <v>1</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F63" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G62" s="3">
+      <c r="G63" s="3">
         <v>92.82</v>
       </c>
-      <c r="H62" s="3">
+      <c r="H63" s="3">
         <v>95.48</v>
       </c>
-      <c r="I62" s="3">
+      <c r="I63" s="3">
         <v>93.67</v>
       </c>
-      <c r="J62" s="3">
+      <c r="J63" s="3">
         <v>86.37</v>
       </c>
-      <c r="K62" s="3">
+      <c r="K63" s="3">
         <v>84.89</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="L63" s="18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B63" s="3">
+      <c r="B64" s="3">
         <v>0.55000000000000004</v>
       </c>
-      <c r="C63" s="3">
-        <v>1</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E63" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F63" t="s">
+      <c r="C64" s="3">
+        <v>1</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E64" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F64" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="G63" s="3">
+      <c r="G64" s="3">
         <v>94.63</v>
       </c>
-      <c r="H63" s="3">
+      <c r="H64" s="3">
         <v>96.79</v>
       </c>
-      <c r="I63" s="3">
+      <c r="I64" s="3">
         <v>94.47</v>
       </c>
-      <c r="J63" s="3">
+      <c r="J64" s="3">
         <v>89.54</v>
       </c>
-      <c r="K63" s="3">
+      <c r="K64" s="3">
         <v>88.56</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+      <c r="L64" s="18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B64" s="3">
+      <c r="B65" s="3">
         <v>0.6</v>
       </c>
-      <c r="C64" s="3">
-        <v>1</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E64" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F64" t="s">
+      <c r="C65" s="3">
+        <v>1</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E65" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F65" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="G64" s="3">
+      <c r="G65" s="3">
         <v>95.56</v>
       </c>
-      <c r="H64" s="3">
+      <c r="H65" s="3">
         <v>97.95</v>
       </c>
-      <c r="I64" s="3">
+      <c r="I65" s="3">
         <v>96.58</v>
       </c>
-      <c r="J64" s="3">
+      <c r="J65" s="3">
         <v>91.92</v>
       </c>
-      <c r="K64" s="3">
+      <c r="K65" s="3">
         <v>91.29</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+      <c r="L65" s="18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B65" s="3">
+      <c r="B66" s="10">
         <v>0.65</v>
       </c>
-      <c r="C65" s="3">
-        <v>1</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E65" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F65" t="s">
+      <c r="C66" s="10">
+        <v>1</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E66" s="10">
+        <v>-1</v>
+      </c>
+      <c r="F66" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="G65" s="3">
+      <c r="G66" s="10">
         <v>96.48</v>
       </c>
-      <c r="H65" s="3">
+      <c r="H66" s="10">
         <v>98.38</v>
       </c>
-      <c r="I65" s="3">
+      <c r="I66" s="10">
         <v>97.22</v>
       </c>
-      <c r="J65" s="3">
+      <c r="J66" s="10">
         <v>93.8</v>
       </c>
-      <c r="K65" s="3">
+      <c r="K66" s="10">
         <v>93.64</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="L66" s="18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B66" s="3">
+      <c r="B67" s="3">
         <v>0.7</v>
       </c>
-      <c r="C66" s="3">
-        <v>1</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E66" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F66" t="s">
+      <c r="C67" s="3">
+        <v>1</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E67" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F67" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="G66" s="3">
+      <c r="G67" s="3">
         <v>97.16</v>
       </c>
-      <c r="H66" s="3">
+      <c r="H67" s="3">
         <v>98.85</v>
       </c>
-      <c r="I66" s="3">
+      <c r="I67" s="3">
         <v>98.05</v>
       </c>
-      <c r="J66" s="3">
+      <c r="J67" s="3">
         <v>95.26</v>
       </c>
-      <c r="K66" s="3">
+      <c r="K67" s="3">
         <v>95.79</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
+      <c r="L67" s="19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B67" s="3">
+      <c r="B68" s="3">
         <v>0.75</v>
       </c>
-      <c r="C67" s="3">
-        <v>1</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E67" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="C68" s="3">
+        <v>1</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E68" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F68" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="G67" s="3">
+      <c r="G68" s="3">
         <v>97.74</v>
       </c>
-      <c r="H67" s="3">
+      <c r="H68" s="3">
         <v>99.16</v>
       </c>
-      <c r="I67" s="3">
+      <c r="I68" s="3">
         <v>98.64</v>
       </c>
-      <c r="J67" s="3">
+      <c r="J68" s="3">
         <v>96.56</v>
       </c>
-      <c r="K67" s="3">
+      <c r="K68" s="3">
         <v>96.76</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
+      <c r="L68" s="19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B69" s="3">
         <v>0.8</v>
       </c>
-      <c r="C68" s="3">
-        <v>1</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E68" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F68" t="s">
+      <c r="C69" s="3">
+        <v>1</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F69" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="G68" s="3">
+      <c r="G69" s="3">
         <v>98.33</v>
       </c>
-      <c r="H68" s="3">
+      <c r="H69" s="3">
         <v>99.4</v>
       </c>
-      <c r="I68" s="3">
+      <c r="I69" s="3">
         <v>99.09</v>
       </c>
-      <c r="J68" s="3">
+      <c r="J69" s="3">
         <v>97.42</v>
       </c>
-      <c r="K68" s="3">
+      <c r="K69" s="3">
         <v>97.68</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+      <c r="L69" s="19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B69" s="3">
+      <c r="B70" s="3">
         <v>0.85</v>
       </c>
-      <c r="C69" s="3">
-        <v>1</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E69" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F69" t="s">
+      <c r="C70" s="3">
+        <v>1</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E70" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F70" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="G69" s="3">
+      <c r="G70" s="3">
         <v>98.88</v>
       </c>
-      <c r="H69" s="3">
+      <c r="H70" s="3">
         <v>99.59</v>
       </c>
-      <c r="I69" s="3">
+      <c r="I70" s="3">
         <v>99.38</v>
       </c>
-      <c r="J69" s="3">
+      <c r="J70" s="3">
         <v>98.43</v>
       </c>
-      <c r="K69" s="3">
+      <c r="K70" s="3">
         <v>98.47</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+      <c r="L70" s="19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B70" s="3">
+      <c r="B71" s="3">
         <v>0.9</v>
       </c>
-      <c r="C70" s="3">
-        <v>1</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E70" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F70" t="s">
+      <c r="C71" s="3">
+        <v>1</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E71" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F71" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="G70" s="3">
+      <c r="G71" s="3">
         <v>99.37</v>
       </c>
-      <c r="H70" s="3">
+      <c r="H71" s="3">
         <v>99.74</v>
       </c>
-      <c r="I70" s="3">
+      <c r="I71" s="3">
         <v>99.54</v>
       </c>
-      <c r="J70" s="3">
+      <c r="J71" s="3">
         <v>99.07</v>
       </c>
-      <c r="K70" s="3">
+      <c r="K71" s="3">
         <v>99.19</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+      <c r="L71" s="19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B71" s="3">
-        <v>1</v>
-      </c>
-      <c r="C71" s="3">
-        <v>1</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E71" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F71" t="s">
+      <c r="B72" s="3">
+        <v>1</v>
+      </c>
+      <c r="C72" s="3">
+        <v>1</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E72" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F72" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G71" s="3">
+      <c r="G72" s="3">
         <v>100</v>
       </c>
-      <c r="H71" s="3">
+      <c r="H72" s="3">
         <v>100</v>
       </c>
-      <c r="I71" s="3">
+      <c r="I72" s="3">
         <v>100</v>
       </c>
-      <c r="J71" s="3">
+      <c r="J72" s="3">
         <v>100</v>
       </c>
-      <c r="K71" s="3">
+      <c r="K72" s="3">
         <v>100</v>
+      </c>
+      <c r="L72" s="19" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4493,7 +4771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6010B3C-372E-4275-ACE4-D17C1964F878}">
   <dimension ref="F1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
@@ -5291,7 +5569,7 @@
       <c r="F35" s="3">
         <v>0.4</v>
       </c>
-      <c r="G35" s="8">
+      <c r="G35" s="7">
         <v>1</v>
       </c>
       <c r="H35" s="3">

</xml_diff>